<commit_message>
Author                       :Ruchi Pareek Description                  :Updated databse schema for tables user, application and applicationcomments Files modified               :SIH-Divergents_DbSchema.xlsx
</commit_message>
<xml_diff>
--- a/DatabaseSchema/SIH-Divergents_DbSchema.xlsx
+++ b/DatabaseSchema/SIH-Divergents_DbSchema.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="42">
   <si>
     <t>User</t>
   </si>
@@ -37,9 +37,6 @@
     <t>SPOCname - varchar</t>
   </si>
   <si>
-    <t>Username - email (varchar)</t>
-  </si>
-  <si>
     <t>column name</t>
   </si>
   <si>
@@ -49,15 +46,9 @@
     <t>foreign key</t>
   </si>
   <si>
-    <t>userId - int auto increment</t>
-  </si>
-  <si>
     <t>applicationId - int auto increment</t>
   </si>
   <si>
-    <t>username -foreign key</t>
-  </si>
-  <si>
     <t>trainingPartnerId</t>
   </si>
   <si>
@@ -131,6 +122,27 @@
   </si>
   <si>
     <t>applicationState - varchar (Submit, Incomplete, draft,approved, rejectednull)</t>
+  </si>
+  <si>
+    <t>isActive - boolean</t>
+  </si>
+  <si>
+    <t>dateOfSubmission</t>
+  </si>
+  <si>
+    <t>userRole</t>
+  </si>
+  <si>
+    <t>userId - email (varchar)</t>
+  </si>
+  <si>
+    <t>Id - int auto increment</t>
+  </si>
+  <si>
+    <t>userId -foreign key</t>
+  </si>
+  <si>
+    <t>commentsId - varchar</t>
   </si>
 </sst>
 </file>
@@ -674,8 +686,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B5:H28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B7" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" topLeftCell="C7" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -689,18 +701,18 @@
   <sheetData>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" t="s">
         <v>7</v>
-      </c>
-      <c r="C5" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B6" s="10" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
@@ -714,21 +726,21 @@
         <v>2</v>
       </c>
       <c r="H10" s="13" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F11" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>13</v>
-      </c>
       <c r="H11" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
@@ -736,13 +748,13 @@
         <v>4</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>12</v>
+        <v>40</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="H12" s="14" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">
@@ -750,119 +762,130 @@
         <v>5</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="H13" s="14" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B14" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D14" s="9"/>
+        <v>38</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>35</v>
+      </c>
       <c r="F14" s="3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="H14" s="14" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B15" s="6" t="s">
         <v>3</v>
       </c>
+      <c r="D15" s="9" t="s">
+        <v>36</v>
+      </c>
       <c r="F15" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H15" s="14" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B16" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H16" s="14" t="s">
         <v>17</v>
-      </c>
-      <c r="H15" s="14" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="F16" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="H16" s="14" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="17" spans="4:8" x14ac:dyDescent="0.25">
       <c r="F17" s="3" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="H17" s="10" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="18" spans="4:8" x14ac:dyDescent="0.25">
       <c r="F18" s="3" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="H18" s="14" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="19" spans="4:8" x14ac:dyDescent="0.25">
       <c r="F19" s="10" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="20" spans="4:8" x14ac:dyDescent="0.25">
       <c r="F20" s="3" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="21" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D21" s="15" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="22" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D22" s="10" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F22" s="12" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="23" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D23" s="5" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="24" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D24" s="5" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="F24" s="10" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="25" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D25" s="2" t="s">
+        <v>41</v>
+      </c>
       <c r="F25" s="8" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="26" spans="4:8" x14ac:dyDescent="0.25">
       <c r="F26" s="8" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="27" spans="4:8" x14ac:dyDescent="0.25">
       <c r="F27" s="8" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="28" spans="4:8" x14ac:dyDescent="0.25">
       <c r="F28" s="8" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Author: Pranjal Kumar Singh Description: Added tables in database schema
</commit_message>
<xml_diff>
--- a/DatabaseSchema/SIH-Divergents_DbSchema.xlsx
+++ b/DatabaseSchema/SIH-Divergents_DbSchema.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="457"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,8 +16,42 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Author</author>
+  </authors>
+  <commentList>
+    <comment ref="H23" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+PMKVY/ Non PMKVY</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="50">
   <si>
     <t>User</t>
   </si>
@@ -82,9 +116,6 @@
     <t>TrainingPartnerQualificationPack</t>
   </si>
   <si>
-    <t>trainingPartnerQualificationPackId</t>
-  </si>
-  <si>
     <t>Center Name - varchar</t>
   </si>
   <si>
@@ -97,9 +128,6 @@
     <t>applicationId - foreign key</t>
   </si>
   <si>
-    <t>qualificationPack - varchar</t>
-  </si>
-  <si>
     <t>JobRole - varchar</t>
   </si>
   <si>
@@ -143,13 +171,43 @@
   </si>
   <si>
     <t>commentsId - varchar</t>
+  </si>
+  <si>
+    <t>Qualification Packs</t>
+  </si>
+  <si>
+    <t>sector</t>
+  </si>
+  <si>
+    <t>qualificationPackName</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>qualificationPackNumber</t>
+  </si>
+  <si>
+    <t>notionalHours</t>
+  </si>
+  <si>
+    <t>entryQualification</t>
+  </si>
+  <si>
+    <t>qualificationPackLocation</t>
+  </si>
+  <si>
+    <t>qualificationPackUploadDate</t>
+  </si>
+  <si>
+    <t>qualificationPackResponse</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -179,8 +237,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="16">
+  <fills count="17">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -268,6 +339,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -299,7 +376,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -344,6 +421,18 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -683,11 +772,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B5:H28"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B5:H29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" topLeftCell="D20" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -731,13 +820,13 @@
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="H11" s="2" t="s">
         <v>19</v>
@@ -748,13 +837,13 @@
         <v>4</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F12" s="3" t="s">
         <v>11</v>
       </c>
       <c r="H12" s="14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">
@@ -762,7 +851,7 @@
         <v>5</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F13" s="3" t="s">
         <v>12</v>
@@ -773,10 +862,10 @@
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B14" s="6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F14" s="3" t="s">
         <v>13</v>
@@ -790,18 +879,18 @@
         <v>3</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F15" s="3" t="s">
         <v>14</v>
       </c>
       <c r="H15" s="14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B16" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="F16" s="3" t="s">
         <v>15</v>
@@ -815,7 +904,7 @@
         <v>16</v>
       </c>
       <c r="H17" s="10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="18" spans="4:8" x14ac:dyDescent="0.25">
@@ -823,73 +912,103 @@
         <v>17</v>
       </c>
       <c r="H18" s="14" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="19" spans="4:8" x14ac:dyDescent="0.25">
       <c r="F19" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="20" spans="4:8" x14ac:dyDescent="0.25">
       <c r="F20" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="21" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D21" s="15" t="s">
-        <v>30</v>
+        <v>28</v>
+      </c>
+      <c r="H21" s="16" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="22" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D22" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F22" s="12" t="s">
         <v>20</v>
       </c>
+      <c r="H22" s="3" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="23" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D23" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>21</v>
+        <v>30</v>
+      </c>
+      <c r="F23" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="H23" s="3" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="24" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D24" s="5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F24" s="10" t="s">
         <v>10</v>
       </c>
+      <c r="H24" s="3" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="25" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D25" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F25" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
+      </c>
+      <c r="H25" s="18" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="26" spans="4:8" x14ac:dyDescent="0.25">
       <c r="F26" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
+      </c>
+      <c r="H26" s="3" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="27" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="F27" s="8" t="s">
-        <v>28</v>
+      <c r="F27" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="H27" s="3" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="28" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="F28" s="8" t="s">
-        <v>31</v>
+      <c r="F28" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="H28" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="29" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="H29" s="3" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Author: Pranjal Kumar Singh Description: Added CSR Funds, Tenders, Tenders Application tables
</commit_message>
<xml_diff>
--- a/DatabaseSchema/SIH-Divergents_DbSchema.xlsx
+++ b/DatabaseSchema/SIH-Divergents_DbSchema.xlsx
@@ -16,42 +16,8 @@
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author>Author</author>
-  </authors>
-  <commentList>
-    <comment ref="H23" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Author:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-PMKVY/ Non PMKVY</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="73">
   <si>
     <t>User</t>
   </si>
@@ -134,9 +100,6 @@
     <t>Scheme - varchar (PMKVY/Non-PMKVY)</t>
   </si>
   <si>
-    <t>undertakingPath</t>
-  </si>
-  <si>
     <t>Application Comments</t>
   </si>
   <si>
@@ -182,9 +145,6 @@
     <t>qualificationPackName</t>
   </si>
   <si>
-    <t>type</t>
-  </si>
-  <si>
     <t>qualificationPackNumber</t>
   </si>
   <si>
@@ -201,13 +161,88 @@
   </si>
   <si>
     <t>qualificationPackResponse</t>
+  </si>
+  <si>
+    <t>CSR Funds</t>
+  </si>
+  <si>
+    <t>organzationName</t>
+  </si>
+  <si>
+    <t>pocName</t>
+  </si>
+  <si>
+    <t>address</t>
+  </si>
+  <si>
+    <t>phone</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>account</t>
+  </si>
+  <si>
+    <t>csrApplicationNumber</t>
+  </si>
+  <si>
+    <t>Tenders</t>
+  </si>
+  <si>
+    <t>tenderNumber</t>
+  </si>
+  <si>
+    <t>tenderTitle</t>
+  </si>
+  <si>
+    <t>department</t>
+  </si>
+  <si>
+    <t>bidStartDate</t>
+  </si>
+  <si>
+    <t>bidEndDate</t>
+  </si>
+  <si>
+    <t>undertakingLocation</t>
+  </si>
+  <si>
+    <t>tenderUploadDate</t>
+  </si>
+  <si>
+    <t>tenderDocumentLocation</t>
+  </si>
+  <si>
+    <t>Tender Application</t>
+  </si>
+  <si>
+    <t>tenderNumber - foreign key</t>
+  </si>
+  <si>
+    <t>organizationName</t>
+  </si>
+  <si>
+    <t>applicationDate</t>
+  </si>
+  <si>
+    <t>tenderApplicationId</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>tenderApplicationResponse</t>
+  </si>
+  <si>
+    <t>tenderApplicationPdfLocation</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -238,20 +273,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="17">
+  <fills count="18">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -296,12 +326,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -345,6 +369,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -381,7 +417,7 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -399,40 +435,40 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -772,11 +808,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B5:H29"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B5:H36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D20" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+    <sheetView tabSelected="1" topLeftCell="B6" workbookViewId="0">
+      <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -797,7 +833,7 @@
       </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="9" t="s">
         <v>6</v>
       </c>
       <c r="C6" t="s">
@@ -811,16 +847,16 @@
       <c r="D10" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="F10" s="11" t="s">
+      <c r="F10" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="H10" s="13" t="s">
+      <c r="H10" s="11" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>9</v>
@@ -836,13 +872,13 @@
       <c r="B12" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="D12" s="10" t="s">
-        <v>38</v>
+      <c r="D12" s="9" t="s">
+        <v>37</v>
       </c>
       <c r="F12" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="H12" s="14" t="s">
+      <c r="H12" s="12" t="s">
         <v>21</v>
       </c>
     </row>
@@ -850,27 +886,27 @@
       <c r="B13" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D13" s="9" t="s">
-        <v>32</v>
+      <c r="D13" s="8" t="s">
+        <v>31</v>
       </c>
       <c r="F13" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="H13" s="14" t="s">
+      <c r="H13" s="12" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B14" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="D14" s="9" t="s">
-        <v>33</v>
+        <v>35</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>32</v>
       </c>
       <c r="F14" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="H14" s="14" t="s">
+      <c r="H14" s="12" t="s">
         <v>15</v>
       </c>
     </row>
@@ -878,137 +914,222 @@
       <c r="B15" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D15" s="9" t="s">
-        <v>34</v>
+      <c r="D15" s="8" t="s">
+        <v>33</v>
       </c>
       <c r="F15" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="H15" s="14" t="s">
+      <c r="H15" s="12" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B16" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F16" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="H16" s="14" t="s">
+      <c r="H16" s="12" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
       <c r="F17" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="H17" s="10" t="s">
+      <c r="H17" s="9" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D18" s="13" t="s">
+        <v>27</v>
+      </c>
       <c r="F18" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H18" s="14" t="s">
+      <c r="H18" s="12" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B19" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="F19" s="9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B20" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="D20" s="5" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="19" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="F19" s="10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="20" spans="4:8" x14ac:dyDescent="0.25">
       <c r="F20" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="21" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D21" s="15" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B21" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H21" s="13" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B22" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F22" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="H22" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B23" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="F23" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="H23" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B24" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="F24" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B25" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="D25" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="F25" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="H25" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B26" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D26" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="F26" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="H26" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D27" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="F27" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="H21" s="16" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="22" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D22" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="F22" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="H22" s="3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="23" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D23" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="F23" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="H23" s="3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="24" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D24" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="F24" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="H24" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="25" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D25" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="F25" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="H25" s="18" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="26" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="F26" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="H26" s="3" t="s">
+      <c r="H27" s="3" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="27" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="F27" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="H27" s="3" t="s">
+    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D28" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="F28" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="H28" s="3" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="28" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="F28" s="17" t="s">
-        <v>49</v>
-      </c>
-      <c r="H28" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="29" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="H29" s="3" t="s">
-        <v>48</v>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B29" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="D29" s="15" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B30" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D30" s="15" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B31" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="D31" s="15" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B32" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="D32" s="15" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B33" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="D33" s="15" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B34" s="16" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B35" s="16" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B36" s="16" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>